<commit_message>
add logic to adjust cell size
</commit_message>
<xml_diff>
--- a/OverAllTatReport.xlsx
+++ b/OverAllTatReport.xlsx
@@ -141,71 +141,104 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AggReportTable" displayName="AggReportTable" ref="A1:D12" headerRowCount="1">
-  <autoFilter ref="A1:D12"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AggReportTable" displayName="AggReportTable" ref="A1:C13" headerRowCount="1">
+  <autoFilter ref="A1:C13"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="Frequency"/>
     <tableColumn id="2" name="Weighted Mean TAT"/>
     <tableColumn id="3" name="Weighted Median TAT"/>
-    <tableColumn id="4" name="None"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TatDetailsTable" displayName="TatDetailsTable" ref="A1:F57" headerRowCount="1">
-  <autoFilter ref="A1:F57"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TatDetailsTable" displayName="TatDetailsTable" ref="A1:E58" headerRowCount="1">
+  <autoFilter ref="A1:E58"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="AuditName"/>
     <tableColumn id="2" name="Frequency"/>
     <tableColumn id="3" name="NoOfFiles"/>
     <tableColumn id="4" name="AvgTAT(Mean)"/>
     <tableColumn id="5" name="TATMedian"/>
-    <tableColumn id="6" name="None"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="PivotedDetails" displayName="PivotedDetails" ref="A1:D12" headerRowCount="1">
-  <autoFilter ref="A1:D12"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="PivotedDetailsTable" displayName="PivotedDetailsTable" ref="A1:Y22" headerRowCount="1">
+  <autoFilter ref="A1:Y22"/>
+  <tableColumns count="25">
     <tableColumn id="1" name="AuditName"/>
-    <tableColumn id="2" name="AvgTAT(Mean)_"/>
-    <tableColumn id="3" name="AvgTAT(Mean)_Adhoc"/>
-    <tableColumn id="4" name="AvgTAT(Mean)_BiWeekly"/>
+    <tableColumn id="2" name="Adhoc (Mean)"/>
+    <tableColumn id="3" name="Adhoc (Median)"/>
+    <tableColumn id="4" name="BiWeekly (Mean)"/>
+    <tableColumn id="5" name="BiWeekly (Median)"/>
+    <tableColumn id="6" name="Daily (Mean)"/>
+    <tableColumn id="7" name="Daily (Median)"/>
+    <tableColumn id="8" name="Daily (Weekdays) (Mean)"/>
+    <tableColumn id="9" name="Daily (Weekdays) (Median)"/>
+    <tableColumn id="10" name="Monthly (Mean)"/>
+    <tableColumn id="11" name="Monthly (Median)"/>
+    <tableColumn id="12" name="N/A (Mean)"/>
+    <tableColumn id="13" name="N/A (Median)"/>
+    <tableColumn id="14" name="Periodic (Mean)"/>
+    <tableColumn id="15" name="Periodic (Median)"/>
+    <tableColumn id="16" name="Quarterly (Mean)"/>
+    <tableColumn id="17" name="Quarterly (Median)"/>
+    <tableColumn id="18" name="SemiAnnual (Mean)"/>
+    <tableColumn id="19" name="SemiAnnual (Median)"/>
+    <tableColumn id="20" name="Weekly (Mean)"/>
+    <tableColumn id="21" name="Weekly (Median)"/>
+    <tableColumn id="22" name="Weekly (Sunday) (Mean)"/>
+    <tableColumn id="23" name="Weekly (Sunday) (Median)"/>
+    <tableColumn id="24" name="Yearly (Mean)"/>
+    <tableColumn id="25" name="Yearly (Median)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="MeanDetails" displayName="MeanDetails" ref="A1:F57" headerRowCount="1">
-  <autoFilter ref="A1:F57"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="MeanDetailstable" displayName="MeanDetailstable" ref="A1:M22" headerRowCount="1">
+  <autoFilter ref="A1:M22"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="AuditName"/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="Adhoc"/>
-    <tableColumn id="4" name="BiWeekly"/>
-    <tableColumn id="5" name="Daily"/>
-    <tableColumn id="6" name="Daily (Weekdays)"/>
+    <tableColumn id="2" name="Adhoc"/>
+    <tableColumn id="3" name="BiWeekly"/>
+    <tableColumn id="4" name="Daily"/>
+    <tableColumn id="5" name="Daily (Weekdays)"/>
+    <tableColumn id="6" name="Monthly"/>
+    <tableColumn id="7" name="N/A"/>
+    <tableColumn id="8" name="Periodic"/>
+    <tableColumn id="9" name="Quarterly"/>
+    <tableColumn id="10" name="SemiAnnual"/>
+    <tableColumn id="11" name="Weekly"/>
+    <tableColumn id="12" name="Weekly (Sunday)"/>
+    <tableColumn id="13" name="Yearly"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="MedianDetails" displayName="MedianDetails" ref="A1:F57" headerRowCount="1">
-  <autoFilter ref="A1:F57"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="MedianDetailsTable" displayName="MedianDetailsTable" ref="A1:M22" headerRowCount="1">
+  <autoFilter ref="A1:M22"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="AuditName"/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="Adhoc"/>
-    <tableColumn id="4" name="BiWeekly"/>
-    <tableColumn id="5" name="Daily"/>
-    <tableColumn id="6" name="Daily (Weekdays)"/>
+    <tableColumn id="2" name="Adhoc"/>
+    <tableColumn id="3" name="BiWeekly"/>
+    <tableColumn id="4" name="Daily"/>
+    <tableColumn id="5" name="Daily (Weekdays)"/>
+    <tableColumn id="6" name="Monthly"/>
+    <tableColumn id="7" name="N/A"/>
+    <tableColumn id="8" name="Periodic"/>
+    <tableColumn id="9" name="Quarterly"/>
+    <tableColumn id="10" name="SemiAnnual"/>
+    <tableColumn id="11" name="Weekly"/>
+    <tableColumn id="12" name="Weekly (Sunday)"/>
+    <tableColumn id="13" name="Yearly"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -507,6 +540,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="24" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -526,76 +564,81 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Adhoc</t>
+        </is>
+      </c>
       <c r="B2" t="n">
-        <v>2.17</v>
+        <v>16.98</v>
       </c>
       <c r="C2" t="n">
-        <v>1.71</v>
+        <v>18.71</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Adhoc</t>
+          <t>BiWeekly</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>16.98</v>
+        <v>1.08</v>
       </c>
       <c r="C3" t="n">
-        <v>18.71</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BiWeekly</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.08</v>
+        <v>0.96</v>
       </c>
       <c r="C4" t="n">
-        <v>1.08</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Daily (Weekdays)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.96</v>
+        <v>13.21</v>
       </c>
       <c r="C5" t="n">
-        <v>0.73</v>
+        <v>13.33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Daily (Weekdays)</t>
+          <t>Monthly</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13.21</v>
+        <v>0.91</v>
       </c>
       <c r="C6" t="n">
-        <v>13.33</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Monthly</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.91</v>
+        <v>0.3</v>
       </c>
       <c r="C7" t="n">
-        <v>1.21</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="8">
@@ -697,6 +740,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="17" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1025,6 +1075,11 @@
           <t>HomeDepot</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C16" t="n">
         <v>231</v>
       </c>
@@ -1146,6 +1201,11 @@
           <t>Kroger</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C22" t="n">
         <v>1984</v>
       </c>
@@ -1330,6 +1390,11 @@
           <t>PetSmart</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
       <c r="C31" t="n">
         <v>4</v>
       </c>
@@ -1617,6 +1682,11 @@
       <c r="A45" t="inlineStr">
         <is>
           <t>Walmart</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1919,10 +1989,38 @@
   <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="7" max="7"/>
+    <col width="28" customWidth="1" min="8" max="8"/>
+    <col width="30" customWidth="1" min="9" max="9"/>
+    <col width="19" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
+    <col width="17" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
+    <col width="22" customWidth="1" min="15" max="15"/>
+    <col width="21" customWidth="1" min="16" max="16"/>
+    <col width="23" customWidth="1" min="17" max="17"/>
+    <col width="22" customWidth="1" min="18" max="18"/>
+    <col width="24" customWidth="1" min="19" max="19"/>
+    <col width="18" customWidth="1" min="20" max="20"/>
+    <col width="20" customWidth="1" min="21" max="21"/>
+    <col width="27" customWidth="1" min="22" max="22"/>
+    <col width="29" customWidth="1" min="23" max="23"/>
+    <col width="18" customWidth="1" min="24" max="24"/>
+    <col width="20" customWidth="1" min="25" max="25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1932,122 +2030,122 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_</t>
+          <t>Adhoc (Mean)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Adhoc</t>
+          <t>Adhoc (Median)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_BiWeekly</t>
+          <t>BiWeekly (Mean)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Daily</t>
+          <t>BiWeekly (Median)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Daily (Weekdays)</t>
+          <t>Daily (Mean)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Monthly</t>
+          <t>Daily (Median)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Periodic</t>
+          <t>Daily (Weekdays) (Mean)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Quarterly</t>
+          <t>Daily (Weekdays) (Median)</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_SemiAnnual</t>
+          <t>Monthly (Mean)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Weekly</t>
+          <t>Monthly (Median)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Weekly (Sunday)</t>
+          <t>N/A (Mean)</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>AvgTAT(Mean)_Yearly</t>
+          <t>N/A (Median)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_</t>
+          <t>Periodic (Mean)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Adhoc</t>
+          <t>Periodic (Median)</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_BiWeekly</t>
+          <t>Quarterly (Mean)</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Daily</t>
+          <t>Quarterly (Median)</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Daily (Weekdays)</t>
+          <t>SemiAnnual (Mean)</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Monthly</t>
+          <t>SemiAnnual (Median)</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Periodic</t>
+          <t>Weekly (Mean)</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Quarterly</t>
+          <t>Weekly (Median)</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_SemiAnnual</t>
+          <t>Weekly (Sunday) (Mean)</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Weekly</t>
+          <t>Weekly (Sunday) (Median)</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Weekly (Sunday)</t>
+          <t>Yearly (Mean)</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>TATMedian_Yearly</t>
+          <t>Yearly (Median)</t>
         </is>
       </c>
     </row>
@@ -2057,16 +2155,16 @@
           <t>Ahold</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.2083</v>
       </c>
-      <c r="K2" t="n">
+      <c r="G2" t="n">
+        <v>0.0417</v>
+      </c>
+      <c r="T2" t="n">
         <v>0.125</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0.0417</v>
-      </c>
-      <c r="W2" t="n">
+      <c r="U2" t="n">
         <v>0.1667</v>
       </c>
     </row>
@@ -2076,16 +2174,16 @@
           <t>Amazon</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>19.0417</v>
+      </c>
       <c r="C3" t="n">
-        <v>19.0417</v>
-      </c>
-      <c r="G3" t="n">
+        <v>18.7083</v>
+      </c>
+      <c r="J3" t="n">
         <v>1.5</v>
       </c>
-      <c r="O3" t="n">
-        <v>18.7083</v>
-      </c>
-      <c r="S3" t="n">
+      <c r="K3" t="n">
         <v>1.2083</v>
       </c>
     </row>
@@ -2095,10 +2193,10 @@
           <t>BestBuy</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>2</v>
       </c>
-      <c r="S4" t="n">
+      <c r="K4" t="n">
         <v>1.6667</v>
       </c>
     </row>
@@ -2108,22 +2206,22 @@
           <t>CVS</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.875</v>
       </c>
       <c r="G5" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J5" t="n">
         <v>12.9583</v>
       </c>
       <c r="K5" t="n">
+        <v>12.9583</v>
+      </c>
+      <c r="T5" t="n">
         <v>4.2917</v>
       </c>
-      <c r="Q5" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="S5" t="n">
-        <v>12.9583</v>
-      </c>
-      <c r="W5" t="n">
+      <c r="U5" t="n">
         <v>4.5833</v>
       </c>
     </row>
@@ -2133,22 +2231,22 @@
           <t>CanadianTire</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1.8333</v>
       </c>
       <c r="G6" t="n">
+        <v>1.4583</v>
+      </c>
+      <c r="J6" t="n">
         <v>7.7083</v>
       </c>
       <c r="K6" t="n">
+        <v>10</v>
+      </c>
+      <c r="T6" t="n">
         <v>1.5833</v>
       </c>
-      <c r="Q6" t="n">
-        <v>1.4583</v>
-      </c>
-      <c r="S6" t="n">
-        <v>10</v>
-      </c>
-      <c r="W6" t="n">
+      <c r="U6" t="n">
         <v>1.25</v>
       </c>
     </row>
@@ -2158,14 +2256,14 @@
           <t>DSG</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="T7" t="n">
         <v>2.0833</v>
       </c>
-      <c r="M7" t="n">
+      <c r="U7" t="n">
+        <v>1.0417</v>
+      </c>
+      <c r="X7" t="n">
         <v>3.9167</v>
-      </c>
-      <c r="W7" t="n">
-        <v>1.0417</v>
       </c>
       <c r="Y7" t="n">
         <v>3.9167</v>
@@ -2177,28 +2275,28 @@
           <t>Delhaize</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>0.4167</v>
+      </c>
       <c r="C8" t="n">
-        <v>0.4167</v>
-      </c>
-      <c r="E8" t="n">
+        <v>0.3333</v>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
       <c r="G8" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J8" t="n">
         <v>0.2917</v>
       </c>
       <c r="K8" t="n">
+        <v>0.2083</v>
+      </c>
+      <c r="T8" t="n">
         <v>2.125</v>
       </c>
-      <c r="O8" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.2083</v>
-      </c>
-      <c r="W8" t="n">
+      <c r="U8" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -2208,16 +2306,16 @@
           <t>GiantEagle</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="J9" t="n">
         <v>5.375</v>
       </c>
       <c r="K9" t="n">
+        <v>0.7083</v>
+      </c>
+      <c r="T9" t="n">
         <v>0.0417</v>
       </c>
-      <c r="S9" t="n">
-        <v>0.7083</v>
-      </c>
-      <c r="W9" t="n">
+      <c r="U9" t="n">
         <v>0.0417</v>
       </c>
     </row>
@@ -2227,22 +2325,22 @@
           <t>HomeDepot</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="H10" t="n">
+        <v>13.2083</v>
+      </c>
+      <c r="I10" t="n">
+        <v>13.3333</v>
+      </c>
+      <c r="L10" t="n">
         <v>2.1667</v>
       </c>
-      <c r="F10" t="n">
-        <v>13.2083</v>
-      </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
+        <v>1.7083</v>
+      </c>
+      <c r="V10" t="n">
         <v>2.6667</v>
       </c>
-      <c r="N10" t="n">
-        <v>1.7083</v>
-      </c>
-      <c r="R10" t="n">
-        <v>13.3333</v>
-      </c>
-      <c r="X10" t="n">
+      <c r="W10" t="n">
         <v>0.9167</v>
       </c>
     </row>
@@ -2252,10 +2350,10 @@
           <t>Ingles</t>
         </is>
       </c>
-      <c r="K11" t="n">
+      <c r="T11" t="n">
         <v>2.4167</v>
       </c>
-      <c r="W11" t="n">
+      <c r="U11" t="n">
         <v>2.4167</v>
       </c>
     </row>
@@ -2265,22 +2363,22 @@
           <t>JCP</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.4583</v>
       </c>
       <c r="G12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J12" t="n">
         <v>7.5417</v>
       </c>
       <c r="K12" t="n">
+        <v>8.083299999999999</v>
+      </c>
+      <c r="T12" t="n">
         <v>0.75</v>
       </c>
-      <c r="Q12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="S12" t="n">
-        <v>8.083299999999999</v>
-      </c>
-      <c r="W12" t="n">
+      <c r="U12" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -2290,22 +2388,28 @@
           <t>Kroger</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>1</v>
       </c>
-      <c r="H13" t="n">
+      <c r="G13" t="n">
+        <v>0.8333</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.0833</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0833</v>
+      </c>
+      <c r="N13" t="n">
         <v>1.5</v>
       </c>
-      <c r="K13" t="n">
+      <c r="O13" t="n">
+        <v>0.5417</v>
+      </c>
+      <c r="T13" t="n">
         <v>0.7917</v>
       </c>
-      <c r="Q13" t="n">
-        <v>0.8333</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0.5417</v>
-      </c>
-      <c r="W13" t="n">
+      <c r="U13" t="n">
         <v>0.7083</v>
       </c>
     </row>
@@ -2315,28 +2419,28 @@
           <t>Loblaws</t>
         </is>
       </c>
+      <c r="B14" t="n">
+        <v>2.25</v>
+      </c>
       <c r="C14" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="E14" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F14" t="n">
         <v>0.6667</v>
       </c>
       <c r="G14" t="n">
+        <v>0.6667</v>
+      </c>
+      <c r="J14" t="n">
         <v>1.3333</v>
       </c>
       <c r="K14" t="n">
+        <v>0.9583</v>
+      </c>
+      <c r="T14" t="n">
         <v>2.625</v>
       </c>
-      <c r="O14" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0.6667</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.9583</v>
-      </c>
-      <c r="W14" t="n">
+      <c r="U14" t="n">
         <v>1.2917</v>
       </c>
     </row>
@@ -2346,16 +2450,16 @@
           <t>Lowes</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="J15" t="n">
         <v>1.25</v>
       </c>
       <c r="K15" t="n">
         <v>1.6667</v>
       </c>
-      <c r="S15" t="n">
+      <c r="T15" t="n">
         <v>1.6667</v>
       </c>
-      <c r="W15" t="n">
+      <c r="U15" t="n">
         <v>1.1667</v>
       </c>
     </row>
@@ -2365,10 +2469,10 @@
           <t>Overwaitea</t>
         </is>
       </c>
-      <c r="K16" t="n">
+      <c r="T16" t="n">
         <v>6.9167</v>
       </c>
-      <c r="W16" t="n">
+      <c r="U16" t="n">
         <v>3.7083</v>
       </c>
     </row>
@@ -2378,10 +2482,16 @@
           <t>PetSmart</t>
         </is>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0.375</v>
       </c>
-      <c r="W17" t="n">
+      <c r="M17" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="U17" t="n">
         <v>0.2083</v>
       </c>
     </row>
@@ -2391,22 +2501,22 @@
           <t>RiteAid</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="J18" t="n">
         <v>0.1667</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
+        <v>0.0417</v>
+      </c>
+      <c r="P18" t="n">
         <v>3.9167</v>
       </c>
-      <c r="K18" t="n">
+      <c r="Q18" t="n">
+        <v>3.9167</v>
+      </c>
+      <c r="T18" t="n">
         <v>0.7083</v>
       </c>
-      <c r="S18" t="n">
-        <v>0.0417</v>
-      </c>
       <c r="U18" t="n">
-        <v>3.9167</v>
-      </c>
-      <c r="W18" t="n">
         <v>0.7083</v>
       </c>
     </row>
@@ -2416,22 +2526,22 @@
           <t>Wakefern</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="J19" t="n">
         <v>5.4583</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
+        <v>5.4583</v>
+      </c>
+      <c r="R19" t="n">
         <v>4.625</v>
       </c>
-      <c r="K19" t="n">
+      <c r="S19" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="T19" t="n">
         <v>1.4167</v>
       </c>
-      <c r="S19" t="n">
-        <v>5.4583</v>
-      </c>
-      <c r="V19" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="W19" t="n">
+      <c r="U19" t="n">
         <v>1.4167</v>
       </c>
     </row>
@@ -2441,28 +2551,28 @@
           <t>Walgreens</t>
         </is>
       </c>
+      <c r="B20" t="n">
+        <v>2.5417</v>
+      </c>
       <c r="C20" t="n">
-        <v>2.5417</v>
-      </c>
-      <c r="E20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F20" t="n">
         <v>0.7083</v>
       </c>
       <c r="G20" t="n">
+        <v>0.7917</v>
+      </c>
+      <c r="J20" t="n">
         <v>1.75</v>
       </c>
       <c r="K20" t="n">
+        <v>1.0417</v>
+      </c>
+      <c r="T20" t="n">
         <v>14.9583</v>
       </c>
-      <c r="O20" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0.7917</v>
-      </c>
-      <c r="S20" t="n">
-        <v>1.0417</v>
-      </c>
-      <c r="W20" t="n">
+      <c r="U20" t="n">
         <v>4.25</v>
       </c>
     </row>
@@ -2472,22 +2582,28 @@
           <t>Walmart</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>0.0833</v>
       </c>
       <c r="G21" t="n">
+        <v>0.0833</v>
+      </c>
+      <c r="J21" t="n">
         <v>0.1667</v>
       </c>
       <c r="K21" t="n">
+        <v>0.1667</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.9167</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.9583</v>
+      </c>
+      <c r="T21" t="n">
         <v>0.0417</v>
       </c>
-      <c r="Q21" t="n">
-        <v>0.0833</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0.1667</v>
-      </c>
-      <c r="W21" t="n">
+      <c r="U21" t="n">
         <v>0.0833</v>
       </c>
     </row>
@@ -2501,24 +2617,24 @@
         <v>1.0833</v>
       </c>
       <c r="E22" t="n">
+        <v>1.0833</v>
+      </c>
+      <c r="F22" t="n">
         <v>2</v>
       </c>
       <c r="G22" t="n">
+        <v>1.9583</v>
+      </c>
+      <c r="J22" t="n">
         <v>2.9583</v>
       </c>
       <c r="K22" t="n">
+        <v>1.6667</v>
+      </c>
+      <c r="T22" t="n">
         <v>1.8333</v>
       </c>
-      <c r="P22" t="n">
-        <v>1.0833</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>1.9583</v>
-      </c>
-      <c r="S22" t="n">
-        <v>1.6667</v>
-      </c>
-      <c r="W22" t="n">
+      <c r="U22" t="n">
         <v>1.6667</v>
       </c>
     </row>
@@ -2543,6 +2659,21 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="13" max="13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2550,30 +2681,34 @@
           <t>AuditName</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Adhoc</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Adhoc</t>
+          <t>BiWeekly</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>BiWeekly</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Daily (Weekdays)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Daily (Weekdays)</t>
+          <t>Monthly</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Monthly</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -2613,7 +2748,7 @@
           <t>Ahold</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>0.2083</v>
       </c>
       <c r="K2" t="n">
@@ -2626,10 +2761,10 @@
           <t>Amazon</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>19.0417</v>
       </c>
-      <c r="G3" t="n">
+      <c r="F3" t="n">
         <v>1.5</v>
       </c>
     </row>
@@ -2639,7 +2774,7 @@
           <t>BestBuy</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="F4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2649,10 +2784,10 @@
           <t>CVS</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>0.875</v>
       </c>
-      <c r="G5" t="n">
+      <c r="F5" t="n">
         <v>12.9583</v>
       </c>
       <c r="K5" t="n">
@@ -2665,10 +2800,10 @@
           <t>CanadianTire</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>1.8333</v>
       </c>
-      <c r="G6" t="n">
+      <c r="F6" t="n">
         <v>7.7083</v>
       </c>
       <c r="K6" t="n">
@@ -2694,13 +2829,13 @@
           <t>Delhaize</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>0.4167</v>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="G8" t="n">
+      <c r="F8" t="n">
         <v>0.2917</v>
       </c>
       <c r="K8" t="n">
@@ -2713,7 +2848,7 @@
           <t>GiantEagle</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="F9" t="n">
         <v>5.375</v>
       </c>
       <c r="K9" t="n">
@@ -2726,11 +2861,11 @@
           <t>HomeDepot</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="E10" t="n">
+        <v>13.2083</v>
+      </c>
+      <c r="G10" t="n">
         <v>2.1667</v>
-      </c>
-      <c r="F10" t="n">
-        <v>13.2083</v>
       </c>
       <c r="L10" t="n">
         <v>2.6667</v>
@@ -2752,10 +2887,10 @@
           <t>JCP</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>0.4583</v>
       </c>
-      <c r="G12" t="n">
+      <c r="F12" t="n">
         <v>7.5417</v>
       </c>
       <c r="K12" t="n">
@@ -2768,8 +2903,11 @@
           <t>Kroger</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0833</v>
       </c>
       <c r="H13" t="n">
         <v>1.5</v>
@@ -2784,13 +2922,13 @@
           <t>Loblaws</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>2.25</v>
       </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>0.6667</v>
       </c>
-      <c r="G14" t="n">
+      <c r="F14" t="n">
         <v>1.3333</v>
       </c>
       <c r="K14" t="n">
@@ -2803,7 +2941,7 @@
           <t>Lowes</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="F15" t="n">
         <v>1.25</v>
       </c>
       <c r="K15" t="n">
@@ -2826,6 +2964,9 @@
           <t>PetSmart</t>
         </is>
       </c>
+      <c r="G17" t="n">
+        <v>0.375</v>
+      </c>
       <c r="K17" t="n">
         <v>0.375</v>
       </c>
@@ -2836,7 +2977,7 @@
           <t>RiteAid</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="F18" t="n">
         <v>0.1667</v>
       </c>
       <c r="I18" t="n">
@@ -2852,7 +2993,7 @@
           <t>Wakefern</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="F19" t="n">
         <v>5.4583</v>
       </c>
       <c r="J19" t="n">
@@ -2868,13 +3009,13 @@
           <t>Walgreens</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="B20" t="n">
         <v>2.5417</v>
       </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>0.7083</v>
       </c>
-      <c r="G20" t="n">
+      <c r="F20" t="n">
         <v>1.75</v>
       </c>
       <c r="K20" t="n">
@@ -2887,11 +3028,14 @@
           <t>Walmart</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>0.0833</v>
       </c>
+      <c r="F21" t="n">
+        <v>0.1667</v>
+      </c>
       <c r="G21" t="n">
-        <v>0.1667</v>
+        <v>0.9167</v>
       </c>
       <c r="K21" t="n">
         <v>0.0417</v>
@@ -2903,13 +3047,13 @@
           <t>WalmartMX</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>1.0833</v>
+      </c>
       <c r="D22" t="n">
-        <v>1.0833</v>
-      </c>
-      <c r="E22" t="n">
         <v>2</v>
       </c>
-      <c r="G22" t="n">
+      <c r="F22" t="n">
         <v>2.9583</v>
       </c>
       <c r="K22" t="n">
@@ -2937,6 +3081,21 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
+    <col width="11" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="11" customWidth="1" min="13" max="13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2944,30 +3103,34 @@
           <t>AuditName</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Adhoc</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Adhoc</t>
+          <t>BiWeekly</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>BiWeekly</t>
+          <t>Daily</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Daily</t>
+          <t>Daily (Weekdays)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Daily (Weekdays)</t>
+          <t>Monthly</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Monthly</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -3007,7 +3170,7 @@
           <t>Ahold</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" t="n">
         <v>0.0417</v>
       </c>
       <c r="K2" t="n">
@@ -3020,10 +3183,10 @@
           <t>Amazon</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>18.7083</v>
       </c>
-      <c r="G3" t="n">
+      <c r="F3" t="n">
         <v>1.2083</v>
       </c>
     </row>
@@ -3033,7 +3196,7 @@
           <t>BestBuy</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="F4" t="n">
         <v>1.6667</v>
       </c>
     </row>
@@ -3043,10 +3206,10 @@
           <t>CVS</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" t="n">
         <v>0.875</v>
       </c>
-      <c r="G5" t="n">
+      <c r="F5" t="n">
         <v>12.9583</v>
       </c>
       <c r="K5" t="n">
@@ -3059,10 +3222,10 @@
           <t>CanadianTire</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" t="n">
         <v>1.4583</v>
       </c>
-      <c r="G6" t="n">
+      <c r="F6" t="n">
         <v>10</v>
       </c>
       <c r="K6" t="n">
@@ -3088,13 +3251,13 @@
           <t>Delhaize</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>0.3333</v>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" t="n">
         <v>0.625</v>
       </c>
-      <c r="G8" t="n">
+      <c r="F8" t="n">
         <v>0.2083</v>
       </c>
       <c r="K8" t="n">
@@ -3107,7 +3270,7 @@
           <t>GiantEagle</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="F9" t="n">
         <v>0.7083</v>
       </c>
       <c r="K9" t="n">
@@ -3120,11 +3283,11 @@
           <t>HomeDepot</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="E10" t="n">
+        <v>13.3333</v>
+      </c>
+      <c r="G10" t="n">
         <v>1.7083</v>
-      </c>
-      <c r="F10" t="n">
-        <v>13.3333</v>
       </c>
       <c r="L10" t="n">
         <v>0.9167</v>
@@ -3146,10 +3309,10 @@
           <t>JCP</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="D12" t="n">
         <v>0.5</v>
       </c>
-      <c r="G12" t="n">
+      <c r="F12" t="n">
         <v>8.083299999999999</v>
       </c>
       <c r="K12" t="n">
@@ -3162,8 +3325,11 @@
           <t>Kroger</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="D13" t="n">
         <v>0.8333</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0833</v>
       </c>
       <c r="H13" t="n">
         <v>0.5417</v>
@@ -3178,13 +3344,13 @@
           <t>Loblaws</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="B14" t="n">
         <v>2.5</v>
       </c>
-      <c r="E14" t="n">
+      <c r="D14" t="n">
         <v>0.6667</v>
       </c>
-      <c r="G14" t="n">
+      <c r="F14" t="n">
         <v>0.9583</v>
       </c>
       <c r="K14" t="n">
@@ -3197,7 +3363,7 @@
           <t>Lowes</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="F15" t="n">
         <v>1.6667</v>
       </c>
       <c r="K15" t="n">
@@ -3220,6 +3386,9 @@
           <t>PetSmart</t>
         </is>
       </c>
+      <c r="G17" t="n">
+        <v>0.125</v>
+      </c>
       <c r="K17" t="n">
         <v>0.2083</v>
       </c>
@@ -3230,7 +3399,7 @@
           <t>RiteAid</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="F18" t="n">
         <v>0.0417</v>
       </c>
       <c r="I18" t="n">
@@ -3246,7 +3415,7 @@
           <t>Wakefern</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="F19" t="n">
         <v>5.4583</v>
       </c>
       <c r="J19" t="n">
@@ -3262,13 +3431,13 @@
           <t>Walgreens</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="B20" t="n">
         <v>0.5</v>
       </c>
-      <c r="E20" t="n">
+      <c r="D20" t="n">
         <v>0.7917</v>
       </c>
-      <c r="G20" t="n">
+      <c r="F20" t="n">
         <v>1.0417</v>
       </c>
       <c r="K20" t="n">
@@ -3281,11 +3450,14 @@
           <t>Walmart</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="D21" t="n">
         <v>0.0833</v>
       </c>
+      <c r="F21" t="n">
+        <v>0.1667</v>
+      </c>
       <c r="G21" t="n">
-        <v>0.1667</v>
+        <v>0.9583</v>
       </c>
       <c r="K21" t="n">
         <v>0.0833</v>
@@ -3297,13 +3469,13 @@
           <t>WalmartMX</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>1.0833</v>
+      </c>
       <c r="D22" t="n">
-        <v>1.0833</v>
-      </c>
-      <c r="E22" t="n">
         <v>1.9583</v>
       </c>
-      <c r="G22" t="n">
+      <c r="F22" t="n">
         <v>1.6667</v>
       </c>
       <c r="K22" t="n">

</xml_diff>